<commit_message>
move to dev mode back
</commit_message>
<xml_diff>
--- a/public/temp/Karyawan.xlsx
+++ b/public/temp/Karyawan.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mada\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05F0FA6D-52E3-4798-927A-3EA1F4D5C7E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E4E45-956C-4121-BB8F-B6BE8A68F62C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37A82FCC-2F1B-4B5F-B795-B091F1AD801C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$325</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1 (2)'!$A$1:$D$312</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>EMP_ID</t>
   </si>
@@ -36,47 +36,116 @@
     <t>dept</t>
   </si>
   <si>
-    <t>1992000035</t>
-  </si>
-  <si>
-    <t>ARIS YULIANTO</t>
-  </si>
-  <si>
-    <t>HR &amp; BOD</t>
-  </si>
-  <si>
-    <t>1992000049</t>
-  </si>
-  <si>
-    <t>KHOLISUL MAJID</t>
-  </si>
-  <si>
-    <t>WD Engineering</t>
-  </si>
-  <si>
-    <t>1992000058</t>
-  </si>
-  <si>
-    <t>LASIM BIN RANTA</t>
-  </si>
-  <si>
-    <t>1992000066</t>
-  </si>
-  <si>
-    <t>OKSEN</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
     <t>RFID</t>
+  </si>
+  <si>
+    <t>DKM 2</t>
+  </si>
+  <si>
+    <t>DKM 3</t>
+  </si>
+  <si>
+    <t>DKM 4</t>
+  </si>
+  <si>
+    <t>DKM 7</t>
+  </si>
+  <si>
+    <t>DKM 8</t>
+  </si>
+  <si>
+    <t>DKM 13</t>
+  </si>
+  <si>
+    <t>TAMU 1</t>
+  </si>
+  <si>
+    <t>TAMU 2</t>
+  </si>
+  <si>
+    <t>TAMU 3</t>
+  </si>
+  <si>
+    <t>TAMU 4</t>
+  </si>
+  <si>
+    <t>TAMU 5</t>
+  </si>
+  <si>
+    <t>fungsi</t>
+  </si>
+  <si>
+    <t>KOPERASI 1 (Agis)</t>
+  </si>
+  <si>
+    <t>KOPERASI 2 (Hendra)</t>
+  </si>
+  <si>
+    <t>ACIM S</t>
+  </si>
+  <si>
+    <t>DKM 1 (Subarkah)</t>
+  </si>
+  <si>
+    <t>DKM 5 (EVI)</t>
+  </si>
+  <si>
+    <t>DKM 6 (Jono)</t>
+  </si>
+  <si>
+    <t>DKM 9 (Roni)</t>
+  </si>
+  <si>
+    <t>DKM 10 (Supiden)</t>
+  </si>
+  <si>
+    <t>DKM 11 (Makhirun)</t>
+  </si>
+  <si>
+    <t>DKM 12 (Nirum)</t>
+  </si>
+  <si>
+    <t>DSS 2 (Hendrianto)</t>
+  </si>
+  <si>
+    <t>DSS 1 (Jajang Nurjaman)</t>
+  </si>
+  <si>
+    <t>DSS 3 (Fauzi)</t>
+  </si>
+  <si>
+    <t>Security (Subcont)</t>
+  </si>
+  <si>
+    <t>Cleaning Service (Subcont)</t>
+  </si>
+  <si>
+    <t>Driver (Subcont)</t>
+  </si>
+  <si>
+    <t>Scrap (Subcont)</t>
+  </si>
+  <si>
+    <t>Koperasi Gobel (Subcont)</t>
+  </si>
+  <si>
+    <t>Klinik (Subcont)</t>
+  </si>
+  <si>
+    <t>Tamu (Subcont)</t>
+  </si>
+  <si>
+    <t>Marbot (Subcont)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +165,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +186,14 @@
         <bgColor indexed="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -160,13 +242,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,12 +268,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet2" xfId="2" xr:uid="{CF6CA40F-9385-4FA7-B7E5-2CC2E6E188DE}"/>
-    <cellStyle name="Normal_Sheet3" xfId="1" xr:uid="{B828EF2D-B1F6-44BA-A760-F8824EFA21FD}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Sheet2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_Sheet3" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,323 +592,558 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644829EF-68C2-47B9-B3D0-9364A5936350}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr transitionEvaluation="1"/>
-  <dimension ref="A1:D325"/>
+  <dimension ref="A1:E312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2020000001</v>
+      </c>
+      <c r="B2" s="5">
+        <v>200001000000</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2020000002</v>
+      </c>
+      <c r="B3" s="5">
+        <v>200002000000</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2020000003</v>
+      </c>
+      <c r="B4" s="5">
+        <v>200003000000</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2020000004</v>
+      </c>
+      <c r="B5" s="5">
+        <v>200004000000</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2020000005</v>
+      </c>
+      <c r="B6" s="5">
+        <v>200005000000</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>920035000000</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2020000006</v>
+      </c>
+      <c r="B7" s="5">
+        <v>200006000000</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2020000007</v>
+      </c>
+      <c r="B8" s="5">
+        <v>200007000000</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2020000008</v>
+      </c>
+      <c r="B9" s="5">
+        <v>200008000000</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2020000009</v>
+      </c>
+      <c r="B10" s="5">
+        <v>200009000000</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2020000010</v>
+      </c>
+      <c r="B11" s="5">
+        <v>200010000000</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2020000011</v>
+      </c>
+      <c r="B12" s="5">
+        <v>200011000000</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2020000012</v>
+      </c>
+      <c r="B13" s="5">
+        <v>200012000000</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2020000013</v>
+      </c>
+      <c r="B14" s="5">
+        <v>200013000000</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2020000014</v>
+      </c>
+      <c r="B15" s="5">
+        <v>200014000000</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2020000015</v>
+      </c>
+      <c r="B16" s="5">
+        <v>200015000000</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2020000016</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200016000000</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2020000017</v>
+      </c>
+      <c r="B18" s="5">
+        <v>200017000000</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5">
-        <v>920049000000</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5">
-        <v>920058000000</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2020000018</v>
+      </c>
+      <c r="B19" s="5">
+        <v>200018000000</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2020000019</v>
+      </c>
+      <c r="B20" s="5">
+        <v>200019000000</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
-        <v>920066000000</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2020000020</v>
+      </c>
+      <c r="B21" s="5">
+        <v>200020000000</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2020000021</v>
+      </c>
+      <c r="B22" s="5">
+        <v>200021000000</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2020000022</v>
+      </c>
+      <c r="B23" s="5">
+        <v>200022000000</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2020000023</v>
+      </c>
+      <c r="B24" s="5">
+        <v>200023000000</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>2020000024</v>
+      </c>
+      <c r="B25" s="5">
+        <v>200024000000</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
@@ -1933,82 +2270,82 @@
       <c r="D231" s="2"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="2"/>
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
-      <c r="D232" s="2"/>
+      <c r="A232" s="3"/>
+      <c r="B232" s="3"/>
+      <c r="C232" s="3"/>
+      <c r="D232" s="3"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="2"/>
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
-      <c r="D233" s="2"/>
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="2"/>
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
-      <c r="D234" s="2"/>
+      <c r="A234" s="3"/>
+      <c r="B234" s="3"/>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
-      <c r="C235" s="2"/>
-      <c r="D235" s="2"/>
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="2"/>
-      <c r="B236" s="2"/>
-      <c r="C236" s="2"/>
-      <c r="D236" s="2"/>
+      <c r="A236" s="3"/>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="2"/>
-      <c r="B237" s="2"/>
-      <c r="C237" s="2"/>
-      <c r="D237" s="2"/>
+      <c r="A237" s="3"/>
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="2"/>
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
-      <c r="D238" s="2"/>
+      <c r="A238" s="3"/>
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="2"/>
-      <c r="B239" s="2"/>
-      <c r="C239" s="2"/>
-      <c r="D239" s="2"/>
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
+      <c r="C239" s="3"/>
+      <c r="D239" s="3"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
-      <c r="D240" s="2"/>
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+      <c r="C240" s="3"/>
+      <c r="D240" s="3"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
-      <c r="D241" s="2"/>
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
+      <c r="C241" s="3"/>
+      <c r="D241" s="3"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
-      <c r="D242" s="2"/>
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
+      <c r="A243" s="3"/>
+      <c r="B243" s="3"/>
+      <c r="C243" s="3"/>
+      <c r="D243" s="3"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
-      <c r="D244" s="2"/>
+      <c r="A244" s="3"/>
+      <c r="B244" s="3"/>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
@@ -2413,86 +2750,8 @@
       <c r="D311" s="3"/>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A312" s="3"/>
-      <c r="B312" s="3"/>
-      <c r="C312" s="3"/>
+      <c r="B312" s="4"/>
       <c r="D312" s="3"/>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A313" s="3"/>
-      <c r="B313" s="3"/>
-      <c r="C313" s="3"/>
-      <c r="D313" s="3"/>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A314" s="3"/>
-      <c r="B314" s="3"/>
-      <c r="C314" s="3"/>
-      <c r="D314" s="3"/>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A315" s="3"/>
-      <c r="B315" s="3"/>
-      <c r="C315" s="3"/>
-      <c r="D315" s="3"/>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A316" s="3"/>
-      <c r="B316" s="3"/>
-      <c r="C316" s="3"/>
-      <c r="D316" s="3"/>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="3"/>
-      <c r="B317" s="3"/>
-      <c r="C317" s="3"/>
-      <c r="D317" s="3"/>
-    </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="3"/>
-      <c r="B318" s="3"/>
-      <c r="C318" s="3"/>
-      <c r="D318" s="3"/>
-    </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="3"/>
-      <c r="B319" s="3"/>
-      <c r="C319" s="3"/>
-      <c r="D319" s="3"/>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A320" s="3"/>
-      <c r="B320" s="3"/>
-      <c r="C320" s="3"/>
-      <c r="D320" s="3"/>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="3"/>
-      <c r="B321" s="3"/>
-      <c r="C321" s="3"/>
-      <c r="D321" s="3"/>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="3"/>
-      <c r="B322" s="3"/>
-      <c r="C322" s="3"/>
-      <c r="D322" s="3"/>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="3"/>
-      <c r="B323" s="3"/>
-      <c r="C323" s="3"/>
-      <c r="D323" s="3"/>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="3"/>
-      <c r="B324" s="3"/>
-      <c r="C324" s="3"/>
-      <c r="D324" s="3"/>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B325" s="4"/>
-      <c r="D325" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>